<commit_message>
soap mandatary fields error fix update
</commit_message>
<xml_diff>
--- a/uploads/dxb_upload_data_31.xlsx
+++ b/uploads/dxb_upload_data_31.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="94">
   <si>
     <t>AIRWAY Bill</t>
   </si>
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A32" sqref="A29:BB32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2318,66 +2318,1735 @@
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>400025541226</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
       <c r="G12" s="2"/>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>38</v>
+      </c>
+      <c r="S12" t="s">
+        <v>39</v>
+      </c>
+      <c r="X12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>0.5</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN12" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AO12" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AP12" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AQ12" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AR12" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AS12" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>400025541215</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
       <c r="G13" s="2"/>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>38</v>
+      </c>
+      <c r="S13" t="s">
+        <v>39</v>
+      </c>
+      <c r="X13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>0.5</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN13" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AO13" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AQ13" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AS13" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY13">
+        <v>0</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="G14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1002880023</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>38</v>
+      </c>
+      <c r="S14" t="s">
+        <v>39</v>
+      </c>
+      <c r="X14" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>4</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN14" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AO14" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AP14" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AQ14" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AR14" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AS14" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="G15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1002880045</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>38</v>
+      </c>
+      <c r="S15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X15" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>3</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN15" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AO15" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AP15" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AQ15" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AR15" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AS15" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY15">
+        <v>0</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA15">
+        <v>0</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1002877352</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" t="s">
+        <v>68</v>
+      </c>
+      <c r="K16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>38</v>
+      </c>
+      <c r="S16" t="s">
+        <v>39</v>
+      </c>
+      <c r="X16" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>3</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AO16" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AP16" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AQ16" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AR16" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AS16" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY16">
+        <v>0</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA16">
+        <v>0</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1002880034</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>38</v>
+      </c>
+      <c r="S17" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>6</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN17" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AO17" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AP17" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AQ17" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AR17" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AS17" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY17">
+        <v>0</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA17">
+        <v>0</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1002880056</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>38</v>
+      </c>
+      <c r="S18" t="s">
+        <v>39</v>
+      </c>
+      <c r="X18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>0.5</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN18" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AO18" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AP18" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AQ18" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AR18" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AS18" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY18">
+        <v>0</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA18">
+        <v>0</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1002880060</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>38</v>
+      </c>
+      <c r="S19" t="s">
+        <v>39</v>
+      </c>
+      <c r="X19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>3</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN19" s="1">
+        <v>43673641</v>
+      </c>
+      <c r="AO19" s="1">
+        <v>43673641</v>
+      </c>
+      <c r="AP19" s="1">
+        <v>43673641</v>
+      </c>
+      <c r="AQ19" s="1">
+        <v>43673641</v>
+      </c>
+      <c r="AR19" s="1">
+        <v>43673641</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>43673641</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY19">
+        <v>0</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA19">
+        <v>0</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1002862556</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
       <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>38</v>
+      </c>
+      <c r="S20" t="s">
+        <v>39</v>
+      </c>
+      <c r="X20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>0.5</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY20">
+        <v>0</v>
+      </c>
+      <c r="AZ20" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA20">
+        <v>0</v>
+      </c>
+      <c r="BB20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1002654741</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>38</v>
+      </c>
+      <c r="S21" t="s">
+        <v>39</v>
+      </c>
+      <c r="X21" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21">
+        <v>0.5</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY21">
+        <v>0</v>
+      </c>
+      <c r="AZ21" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA21">
+        <v>0</v>
+      </c>
+      <c r="BB21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>400025541226</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
       <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L22" t="s">
+        <v>35</v>
+      </c>
+      <c r="M22" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>38</v>
+      </c>
+      <c r="S22" t="s">
+        <v>39</v>
+      </c>
+      <c r="X22" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AC22">
+        <v>0.5</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN22" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AO22" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AP22" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AQ22" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AR22" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AS22" s="1">
+        <v>506304179</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY22">
+        <v>0</v>
+      </c>
+      <c r="AZ22" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA22">
+        <v>0</v>
+      </c>
+      <c r="BB22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>400025541215</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" t="s">
+        <v>51</v>
+      </c>
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>38</v>
+      </c>
+      <c r="S23" t="s">
+        <v>39</v>
+      </c>
+      <c r="X23" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB23">
+        <v>1</v>
+      </c>
+      <c r="AC23">
+        <v>0.5</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN23" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AO23" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AP23" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AQ23" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AR23" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AS23" s="1">
+        <v>43201112</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY23">
+        <v>0</v>
+      </c>
+      <c r="AZ23" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA23">
+        <v>0</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1002880023</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24" t="s">
+        <v>35</v>
+      </c>
+      <c r="M24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>38</v>
+      </c>
+      <c r="S24" t="s">
+        <v>39</v>
+      </c>
+      <c r="X24" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
+        <v>4</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN24" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AO24" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AP24" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AQ24" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AR24" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AS24" s="1">
+        <v>45135880</v>
+      </c>
+      <c r="AT24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY24">
+        <v>0</v>
+      </c>
+      <c r="AZ24" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA24">
+        <v>0</v>
+      </c>
+      <c r="BB24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1002880045</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" t="s">
+        <v>35</v>
+      </c>
+      <c r="M25" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" t="s">
+        <v>35</v>
+      </c>
+      <c r="O25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>38</v>
+      </c>
+      <c r="S25" t="s">
+        <v>39</v>
+      </c>
+      <c r="X25" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>3</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN25" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AO25" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AP25" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AQ25" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AR25" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AS25" s="1">
+        <v>2265640</v>
+      </c>
+      <c r="AT25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX25" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY25">
+        <v>0</v>
+      </c>
+      <c r="AZ25" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA25">
+        <v>0</v>
+      </c>
+      <c r="BB25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1002877352</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26" t="s">
+        <v>35</v>
+      </c>
+      <c r="M26" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" t="s">
+        <v>35</v>
+      </c>
+      <c r="O26" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>38</v>
+      </c>
+      <c r="S26" t="s">
+        <v>39</v>
+      </c>
+      <c r="X26" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB26">
+        <v>1</v>
+      </c>
+      <c r="AC26">
+        <v>3</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN26" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AO26" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AP26" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AQ26" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AR26" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AS26" s="1">
+        <v>42837444</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY26">
+        <v>0</v>
+      </c>
+      <c r="AZ26" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA26">
+        <v>0</v>
+      </c>
+      <c r="BB26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1002880034</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" t="s">
+        <v>51</v>
+      </c>
+      <c r="L27" t="s">
+        <v>35</v>
+      </c>
+      <c r="M27" t="s">
+        <v>36</v>
+      </c>
+      <c r="N27" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>38</v>
+      </c>
+      <c r="S27" t="s">
+        <v>39</v>
+      </c>
+      <c r="X27" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>6</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN27" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AO27" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AP27" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AQ27" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AR27" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AS27" s="1">
+        <v>43980722</v>
+      </c>
+      <c r="AT27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX27" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY27">
+        <v>0</v>
+      </c>
+      <c r="AZ27" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA27">
+        <v>0</v>
+      </c>
+      <c r="BB27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1002880056</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K28" t="s">
+        <v>51</v>
+      </c>
+      <c r="L28" t="s">
+        <v>35</v>
+      </c>
+      <c r="M28" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28" t="s">
+        <v>35</v>
+      </c>
+      <c r="O28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>38</v>
+      </c>
+      <c r="S28" t="s">
+        <v>39</v>
+      </c>
+      <c r="X28" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+      <c r="AC28">
+        <v>0.5</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN28" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AO28" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AP28" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AQ28" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AR28" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AS28" s="1">
+        <v>44063138</v>
+      </c>
+      <c r="AT28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY28">
+        <v>0</v>
+      </c>
+      <c r="AZ28" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA28">
+        <v>0</v>
+      </c>
+      <c r="BB28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.3">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.3">
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.3">
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.3">
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.3">

</xml_diff>